<commit_message>
Structural Analysis of Chadnimukha Begins
Structural Analysis of Chadnimukha Begins
</commit_message>
<xml_diff>
--- a/AE Sakib/Satkhira DIV-I/2021-22/Satkhira-1/Chadnimukha/Input Output/Chadnumukha_input.xlsx
+++ b/AE Sakib/Satkhira DIV-I/2021-22/Satkhira-1/Chadnimukha/Input Output/Chadnumukha_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8136" tabRatio="637" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8136" tabRatio="637" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,13 @@
     <sheet name="Return_wall_data" sheetId="6" r:id="rId6"/>
     <sheet name="Return_wall_data_MKS" sheetId="7" r:id="rId7"/>
     <sheet name="Wing_Wall_Data" sheetId="8" r:id="rId8"/>
-    <sheet name="Regulator_plan" sheetId="9" r:id="rId9"/>
+    <sheet name="Foundation_Pressure_Calcualtion" sheetId="10" r:id="rId9"/>
+    <sheet name="Structural_Design_Parameter" sheetId="11" r:id="rId10"/>
+    <sheet name="Flexure_Design" sheetId="12" r:id="rId11"/>
+    <sheet name="Regulator_plan" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">Regulator_plan!$A$1:$E$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">Regulator_plan!$A$1:$E$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="194">
   <si>
     <t>parameters</t>
   </si>
@@ -179,9 +182,6 @@
     <t>return wall level</t>
   </si>
   <si>
-    <t>fee-pwd</t>
-  </si>
-  <si>
     <t>Top of Appron</t>
   </si>
   <si>
@@ -450,6 +450,171 @@
   </si>
   <si>
     <t>Chadnimukha_2V_DFR</t>
+  </si>
+  <si>
+    <t>Glacis Level</t>
+  </si>
+  <si>
+    <t>Maximum Probable Soil Height</t>
+  </si>
+  <si>
+    <t>Maximum Probable Soil Pressure</t>
+  </si>
+  <si>
+    <t>psf</t>
+  </si>
+  <si>
+    <t>Unit Weight of Soil</t>
+  </si>
+  <si>
+    <t>kpa to psf</t>
+  </si>
+  <si>
+    <t>unit less</t>
+  </si>
+  <si>
+    <t>Maximum Probable Soil Pressure in Kpa</t>
+  </si>
+  <si>
+    <t>kpa to t/sqm</t>
+  </si>
+  <si>
+    <t>Elevation at Which Silt and Fine Sand Found</t>
+  </si>
+  <si>
+    <t>Top of Sand Pile</t>
+  </si>
+  <si>
+    <t>Length of Sand Pile</t>
+  </si>
+  <si>
+    <t>After Rounding</t>
+  </si>
+  <si>
+    <t>Kpa</t>
+  </si>
+  <si>
+    <t>Maximum Probable Soil Pressure (t/sqm)</t>
+  </si>
+  <si>
+    <t>Fine Sand and Clay Safe Bearing Capacity(t/sqm)</t>
+  </si>
+  <si>
+    <t>page 6-45 CIDA  1993 volume2</t>
+  </si>
+  <si>
+    <t>f'c</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>Mpa</t>
+  </si>
+  <si>
+    <t>concete compressive strength Mks</t>
+  </si>
+  <si>
+    <t>Mpa to psi</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>fc</t>
+  </si>
+  <si>
+    <t>allowable compress stress in concrete</t>
+  </si>
+  <si>
+    <t>Vc</t>
+  </si>
+  <si>
+    <t>concrete allowable stress in shear without web reinforcement</t>
+  </si>
+  <si>
+    <t>concrete allowable stress in shear  web reinforcement</t>
+  </si>
+  <si>
+    <t>allowable punching shear stress</t>
+  </si>
+  <si>
+    <t>fy</t>
+  </si>
+  <si>
+    <t>steel yield stress</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>allowable stress in reinforcing steel</t>
+  </si>
+  <si>
+    <t>Es</t>
+  </si>
+  <si>
+    <t>Ec</t>
+  </si>
+  <si>
+    <t>Modulus of Elasticity  of Reinforcing Steel</t>
+  </si>
+  <si>
+    <t>Modulus of Elasticity  of Concrete</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Design Constants:</t>
+  </si>
+  <si>
+    <t>Material Properties:</t>
+  </si>
+  <si>
+    <t>modular ratio</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>allowable stress ratio</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Member Name</t>
+  </si>
+  <si>
+    <t>Top Slab</t>
+  </si>
+  <si>
+    <t>Moment Designation</t>
+  </si>
+  <si>
+    <t>+ Moment(Bottom Tension)</t>
+  </si>
+  <si>
+    <t>Design Moment(Kip-feet/feet)</t>
+  </si>
+  <si>
+    <t>Design Moment(lb-inch/feet)</t>
+  </si>
+  <si>
+    <t>(-) Moment Top Tension</t>
+  </si>
+  <si>
+    <t>t(inch)</t>
+  </si>
+  <si>
+    <t>cc</t>
   </si>
 </sst>
 </file>
@@ -530,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,6 +719,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,6 +1020,852 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="58.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="3">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="3">
+        <v>145.04</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="3">
+        <f>C3*C4</f>
+        <v>3626</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="3">
+        <f>0.4*C5</f>
+        <v>1450.4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="3">
+        <f>1.1*SQRT(C5)</f>
+        <v>66.23790455622823</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="3">
+        <f>5*SQRT(C5)</f>
+        <v>301.08138434649197</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="3">
+        <f>2*SQRT(C5)</f>
+        <v>120.43255373859678</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="3">
+        <v>415</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="3">
+        <f>C10*C4</f>
+        <v>60191.6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="3">
+        <v>24000</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="10">
+        <f>29000*1000</f>
+        <v>29000000</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="10">
+        <f>57000*SQRT(C5)</f>
+        <v>3432327.7815500083</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="3">
+        <f>C13/C14</f>
+        <v>8.4490765001773411</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="3">
+        <f>C12/C6</f>
+        <v>16.54715940430226</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="3">
+        <f>ROUND(C6/((C12/C16)+C6),3)</f>
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="3">
+        <f>ROUND((1-(1/3)*C18),3)</f>
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="3">
+        <f>0.5*C6*C18*C19</f>
+        <v>217.41931120000004</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2*12000</f>
+        <v>43200</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7.24</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3*12000</f>
+        <v>86880</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="205" zoomScaleNormal="115" zoomScaleSheetLayoutView="205" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-2.4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-1.5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="8">
+        <v>-2.5499999999999998</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.95</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="3">
+        <v>12.25</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3">
+        <v>11</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2.98</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="1">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -862,375 +1882,410 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>4.18</v>
       </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>4.92</v>
       </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>12.956</v>
       </c>
+      <c r="D4" s="3"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>-4.92</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f>C4-C11</f>
         <v>17.875999999999998</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>-4.5919999999999996</v>
       </c>
+      <c r="D6" s="3"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>18.04</v>
       </c>
+      <c r="D7" s="3"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>19.68</v>
       </c>
+      <c r="D8" s="3"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>2</v>
       </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
         <v>3</v>
       </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="8">
         <v>-4.92</v>
       </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>54</v>
       </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>2</v>
       </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>5</v>
       </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>6</v>
       </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>9.84</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="3">
         <v>21.32</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1">
+      <c r="B25" s="9"/>
+      <c r="C25" s="3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <v>17.876000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1">
+      <c r="B27" s="9"/>
+      <c r="C27" s="3">
         <v>0.14299999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3">
         <v>3.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="C32" s="8">
+        <v>11.5</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="3">
         <v>12.956</v>
       </c>
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1455,7 +2510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1471,7 +2526,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1484,7 +2539,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1505,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1">
         <v>4.55</v>
@@ -1513,10 +2568,10 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>-8.3640000000000008</v>
@@ -1529,10 +2584,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>8.1999999999999993</v>
@@ -1541,77 +2596,77 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1">
         <v>0.3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1">
         <v>0.17499999999999999</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>0.17499999999999999</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>0.56999999999999995</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>0.39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -1620,12 +2675,12 @@
         <v>14.923999999999999</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -1635,12 +2690,12 @@
         <v>10.036799999999999</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -1649,12 +2704,12 @@
         <v>4.8639999999999999</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
@@ -1663,21 +2718,21 @@
         <v>4.8639999999999999</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>0.33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1689,7 +2744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1711,15 +2766,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>-2.5499999999999998</v>
@@ -1728,10 +2783,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>2.5</v>
@@ -1740,94 +2795,94 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1">
         <v>0.3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1">
         <v>0.17499999999999999</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>0.17499999999999999</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>0.56999999999999995</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>0.39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1">
         <v>4.55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1">
         <v>3.06</v>
@@ -1836,10 +2891,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1">
         <v>1.49</v>
@@ -1848,10 +2903,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1">
         <v>1.7</v>
@@ -1860,16 +2915,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>0.33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1903,15 +2958,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>-8.3640000000000008</v>
@@ -1920,10 +2975,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>12.956</v>
@@ -1932,7 +2987,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
@@ -1941,12 +2996,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -1955,7 +3010,7 @@
         <v>2.67</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1">
         <v>0.17499999999999999</v>
@@ -1963,7 +3018,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
@@ -1972,7 +3027,7 @@
         <v>2.67</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="1">
         <v>0.17499999999999999</v>
@@ -1980,7 +3035,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -1989,7 +3044,7 @@
         <v>39.36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1">
         <v>0.56999999999999995</v>
@@ -1997,7 +3052,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
@@ -2006,7 +3061,7 @@
         <v>14.923999999999999</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="1">
         <v>0.39</v>
@@ -2014,7 +3069,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -2024,12 +3079,12 @@
         <v>10.036799999999999</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -2039,12 +3094,12 @@
         <v>4.8872</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -2054,21 +3109,21 @@
         <v>5.5759999999999996</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1">
         <v>0.33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2078,478 +3133,229 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="205" zoomScaleNormal="115" zoomScaleSheetLayoutView="205" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>18.04</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-4.92</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-4</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <f>C3+C4</f>
+        <v>-8.92</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <f>C2-C5</f>
+        <v>26.96</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3">
+        <v>120</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="3">
+        <f>C6*C7</f>
+        <v>3235.2000000000003</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="3">
+        <v>20.888999999999999</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C8/C9</f>
+        <v>154.87577193738332</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
+        <f>C10/C11</f>
+        <v>15.803650197692175</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-12.17</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-3.7749999999999999</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="3">
-        <v>-2.4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C16" s="3">
+        <f>C15-C14</f>
+        <v>8.3949999999999996</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="3">
-        <v>-1.5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="8">
-        <v>-2.5499999999999998</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3.95</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2.15</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="3">
-        <v>12.25</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="3">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.79</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2.54</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="7">
-        <v>2.98</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="1">
-        <v>25</v>
-      </c>
+      <c r="C17" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="D17" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>